<commit_message>
Update project with test data
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,21 +14,231 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Points</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Kelly</t>
-  </si>
-  <si>
-    <t>Paul Such Co.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Current Points</t>
+  </si>
+  <si>
+    <t>Final Points</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>JJ</t>
+  </si>
+  <si>
+    <t>KK</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>QQ</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>UU</t>
+  </si>
+  <si>
+    <t>VV</t>
+  </si>
+  <si>
+    <t>WW</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>YY</t>
+  </si>
+  <si>
+    <t>ZZ</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>BBB</t>
+  </si>
+  <si>
+    <t>CCC</t>
+  </si>
+  <si>
+    <t>DDD</t>
+  </si>
+  <si>
+    <t>EEE</t>
+  </si>
+  <si>
+    <t>GGG</t>
+  </si>
+  <si>
+    <t>HHH</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>JJJ</t>
+  </si>
+  <si>
+    <t>KKK</t>
+  </si>
+  <si>
+    <t>NNN</t>
+  </si>
+  <si>
+    <t>PPP</t>
+  </si>
+  <si>
+    <t>RRR</t>
+  </si>
+  <si>
+    <t>SSS</t>
+  </si>
+  <si>
+    <t>TTT</t>
+  </si>
+  <si>
+    <t>UUU</t>
+  </si>
+  <si>
+    <t>VVV</t>
+  </si>
+  <si>
+    <t>WWW</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>YYY</t>
+  </si>
+  <si>
+    <t>ZZZ</t>
+  </si>
+  <si>
+    <t>AAAA</t>
+  </si>
+  <si>
+    <t>CCCC</t>
+  </si>
+  <si>
+    <t>DDDD</t>
+  </si>
+  <si>
+    <t>EEEE</t>
+  </si>
+  <si>
+    <t>FFFF</t>
+  </si>
+  <si>
+    <t>GGGG</t>
+  </si>
+  <si>
+    <t>Test Student</t>
   </si>
 </sst>
 </file>
@@ -386,51 +596,1029 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5.5</v>
+      </c>
+      <c r="D3">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>4.5</v>
+      </c>
+      <c r="D4">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>2.5</v>
+      </c>
+      <c r="D10">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>5.5</v>
+      </c>
+      <c r="D14">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>5.5</v>
+      </c>
+      <c r="D15">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>7.5</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28">
+        <v>1.5</v>
+      </c>
+      <c r="D28">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>6.5</v>
+      </c>
+      <c r="D29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30">
+        <v>5.5</v>
+      </c>
+      <c r="D30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32">
+        <v>2.5</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33">
+        <v>7.5</v>
+      </c>
+      <c r="D33">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>42</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>43</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37">
+        <v>8.5</v>
+      </c>
+      <c r="D37">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>45</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>46</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>47</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>48</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41">
+        <v>6.5</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>49</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>50</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>51</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>52</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>53</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>54</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>55</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>56</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49">
+        <v>5.5</v>
+      </c>
+      <c r="D49">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>57</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
+      </c>
+      <c r="D50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>59</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
+      </c>
+      <c r="D51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>60</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52">
+        <v>7</v>
+      </c>
+      <c r="D52">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>61</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>62</v>
+      </c>
+      <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>63</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55">
+        <v>6</v>
+      </c>
+      <c r="D55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>66</v>
+      </c>
+      <c r="B56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1">
+        <v>68</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1">
+        <v>70</v>
+      </c>
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
+      </c>
+      <c r="D58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1">
+        <v>71</v>
+      </c>
+      <c r="B59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59">
+        <v>1.5</v>
+      </c>
+      <c r="D59">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1">
+        <v>72</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60">
+        <v>8.5</v>
+      </c>
+      <c r="D60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1">
+        <v>73</v>
+      </c>
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61">
+        <v>6</v>
+      </c>
+      <c r="D61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1">
+        <v>74</v>
+      </c>
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62">
+        <v>6</v>
+      </c>
+      <c r="D62">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1">
+        <v>75</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+      <c r="D63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1">
+        <v>76</v>
+      </c>
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64">
+        <v>5.5</v>
+      </c>
+      <c r="D64">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
+        <v>77</v>
+      </c>
+      <c r="B65" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
+      <c r="D65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1">
+        <v>78</v>
+      </c>
+      <c r="B66" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66">
+        <v>6.5</v>
+      </c>
+      <c r="D66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
+        <v>79</v>
+      </c>
+      <c r="B67" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67">
+        <v>7.5</v>
+      </c>
+      <c r="D67">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
+        <v>81</v>
+      </c>
+      <c r="B68" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1">
+        <v>82</v>
+      </c>
+      <c r="B69" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69">
+        <v>7</v>
+      </c>
+      <c r="D69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1">
+        <v>83</v>
+      </c>
+      <c r="B70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C70">
+        <v>7</v>
+      </c>
+      <c r="D70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1">
+        <v>84</v>
+      </c>
+      <c r="B71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C71">
+        <v>7</v>
+      </c>
+      <c r="D71">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="1">
+        <v>85</v>
+      </c>
+      <c r="B72" t="s">
+        <v>73</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="1">
+        <v>86</v>
+      </c>
+      <c r="B73" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73">
+        <v>0.5</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>